<commit_message>
EDIT: 2014 Summer resume
</commit_message>
<xml_diff>
--- a/assets/content/2014Summer.xlsx
+++ b/assets/content/2014Summer.xlsx
@@ -192,9 +192,6 @@
     <t>Gradle Build Tool.</t>
   </si>
   <si>
-    <t>Leading group of 14 students in Android Development Course.</t>
-  </si>
-  <si>
     <t>GAME DEVELOPMENT IN JAVA</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
       </rPr>
       <t>http://hangtime.com</t>
     </r>
+  </si>
+  <si>
+    <t>Leading group of 20+ students in Android Development Course.</t>
   </si>
 </sst>
 </file>
@@ -561,6 +561,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -574,9 +577,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -888,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,12 +932,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="5" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
@@ -950,10 +950,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="41"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -961,7 +961,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="35"/>
     </row>
@@ -969,7 +969,7 @@
       <c r="A8" s="31"/>
       <c r="B8" s="3"/>
       <c r="C8" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>3</v>
@@ -979,7 +979,7 @@
       <c r="A9" s="31"/>
       <c r="B9" s="34"/>
       <c r="C9" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="13"/>
     </row>
@@ -995,12 +995,12 @@
       <c r="A11" s="31"/>
       <c r="B11" s="3"/>
       <c r="C11" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="2"/>
@@ -1012,18 +1012,18 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="37" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="42" t="s">
-        <v>47</v>
       </c>
       <c r="D14" s="15"/>
     </row>
@@ -1041,7 +1041,7 @@
       <c r="A16" s="27"/>
       <c r="B16" s="4"/>
       <c r="C16" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="16"/>
     </row>
@@ -1080,7 +1080,7 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="3"/>
       <c r="C21" s="18" t="s">
         <v>28</v>
@@ -1088,7 +1088,7 @@
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="4"/>
       <c r="C22" s="28" t="s">
         <v>22</v>
@@ -1096,7 +1096,7 @@
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="3"/>
       <c r="C23" s="25" t="s">
         <v>7</v>
@@ -1106,12 +1106,12 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="3"/>
       <c r="C24" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="40"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
@@ -1119,7 +1119,7 @@
       <c r="C25" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="41"/>
     </row>
     <row r="26" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
@@ -1127,7 +1127,7 @@
       <c r="C26" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="40"/>
+      <c r="D26" s="41"/>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
@@ -1140,20 +1140,20 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="3"/>
       <c r="C28" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="37"/>
+      <c r="D28" s="38"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="3"/>
       <c r="C29" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="37"/>
+      <c r="D29" s="38"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>34</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C37" s="14" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>